<commit_message>
Rebrand to Forest Inventory Applications
- Update ecosystem tagline in README.md
- Add R&D affiliation section to README.md
- Update docs/index.md footer

Changes ecosystem branding from "Forest Inventory Analysis" to
"Forest Inventory Applications" to avoid confusion with the official
USDA Forest Inventory AND Analysis program.
</commit_message>
<xml_diff>
--- a/test_output/integration_tests/scenario_comparison.xlsx
+++ b/test_output/integration_tests/scenario_comparison.xlsx
@@ -516,13 +516,13 @@
         <v>500</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6953186109445383</v>
+        <v>0.7202346731898849</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5049440163758098</v>
+        <v>0.513911475849385</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4946042510795484</v>
+        <v>0.5044358179472358</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -531,10 +531,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05541344818078302</v>
+        <v>0.05739913488953671</v>
       </c>
       <c r="H2" t="n">
-        <v>4.146440031523783</v>
+        <v>4.265262369620648</v>
       </c>
       <c r="I2" t="n">
         <v>480</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>93.60871057459217</v>
+        <v>93.62013125626211</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -562,40 +562,40 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="B3" t="n">
-        <v>21.87690844866038</v>
+        <v>22.20308141284221</v>
       </c>
       <c r="C3" t="n">
-        <v>2.878767554138274</v>
+        <v>2.879401224404767</v>
       </c>
       <c r="D3" t="n">
-        <v>2.878733961069451</v>
+        <v>2.879374177297288</v>
       </c>
       <c r="E3" t="n">
-        <v>22.63607222640232</v>
+        <v>22.63580122526506</v>
       </c>
       <c r="F3" t="n">
-        <v>22.56402073760179</v>
+        <v>22.56889308861816</v>
       </c>
       <c r="G3" t="n">
-        <v>1.743481209324728</v>
+        <v>1.769475578473134</v>
       </c>
       <c r="H3" t="n">
-        <v>65.59518381229476</v>
+        <v>66.56738536087609</v>
       </c>
       <c r="I3" t="n">
         <v>480</v>
       </c>
       <c r="J3" t="n">
-        <v>1.366566329422807</v>
+        <v>1.386820528351585</v>
       </c>
       <c r="K3" t="n">
         <v>5</v>
       </c>
       <c r="L3" t="n">
-        <v>316.5787019428871</v>
+        <v>321.3059620113886</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -611,40 +611,40 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B4" t="n">
-        <v>53.24853048768503</v>
+        <v>53.47293081480863</v>
       </c>
       <c r="C4" t="n">
-        <v>4.519352019475456</v>
+        <v>4.5194197665066</v>
       </c>
       <c r="D4" t="n">
-        <v>4.519079721189682</v>
+        <v>4.519151007196385</v>
       </c>
       <c r="E4" t="n">
-        <v>36.09470248766853</v>
+        <v>36.09277117852089</v>
       </c>
       <c r="F4" t="n">
-        <v>36.02539560863328</v>
+        <v>36.0284581218981</v>
       </c>
       <c r="G4" t="n">
-        <v>2.934386867273598</v>
+        <v>2.946718756668255</v>
       </c>
       <c r="H4" t="n">
-        <v>133.6057503117547</v>
+        <v>134.1679981583152</v>
       </c>
       <c r="I4" t="n">
         <v>480</v>
       </c>
       <c r="J4" t="n">
-        <v>2.783453131494891</v>
+        <v>2.795166628298233</v>
       </c>
       <c r="K4" t="n">
         <v>10</v>
       </c>
       <c r="L4" t="n">
-        <v>968.5181391414436</v>
+        <v>972.6668686620575</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -660,43 +660,43 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B5" t="n">
-        <v>95.83980130511063</v>
+        <v>95.00177720403157</v>
       </c>
       <c r="C5" t="n">
-        <v>6.107996846100028</v>
+        <v>6.107222321845692</v>
       </c>
       <c r="D5" t="n">
-        <v>6.106322208018327</v>
+        <v>6.10554479002972</v>
       </c>
       <c r="E5" t="n">
-        <v>48.32017906864004</v>
+        <v>48.31721644460434</v>
       </c>
       <c r="F5" t="n">
-        <v>48.24856042605608</v>
+        <v>48.25153233423276</v>
       </c>
       <c r="G5" t="n">
-        <v>4.239443224112956</v>
+        <v>4.202724579741611</v>
       </c>
       <c r="H5" t="n">
-        <v>213.495383122743</v>
+        <v>211.6391785164422</v>
       </c>
       <c r="I5" t="n">
         <v>480</v>
       </c>
       <c r="J5" t="n">
-        <v>4.447820481723814</v>
+        <v>4.409149552425879</v>
       </c>
       <c r="K5" t="n">
         <v>15</v>
       </c>
       <c r="L5" t="n">
-        <v>2207.608931420314</v>
+        <v>2188.437981188561</v>
       </c>
       <c r="M5" t="n">
-        <v>619.5831159857911</v>
+        <v>614.0344210662722</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -709,43 +709,43 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B6" t="n">
-        <v>138.2519505363138</v>
+        <v>137.8001182480799</v>
       </c>
       <c r="C6" t="n">
-        <v>7.407146788814566</v>
+        <v>7.411091660251636</v>
       </c>
       <c r="D6" t="n">
-        <v>7.401643667966121</v>
+        <v>7.405522824688475</v>
       </c>
       <c r="E6" t="n">
-        <v>58.02806327000106</v>
+        <v>58.02817591230716</v>
       </c>
       <c r="F6" t="n">
-        <v>57.95362926591102</v>
+        <v>57.95892898370582</v>
       </c>
       <c r="G6" t="n">
-        <v>5.42652681540639</v>
+        <v>5.407108944112923</v>
       </c>
       <c r="H6" t="n">
-        <v>285.3854006305906</v>
+        <v>284.3928922783617</v>
       </c>
       <c r="I6" t="n">
         <v>480</v>
       </c>
       <c r="J6" t="n">
-        <v>5.945529179803971</v>
+        <v>5.924851922465868</v>
       </c>
       <c r="K6" t="n">
         <v>20</v>
       </c>
       <c r="L6" t="n">
-        <v>3759.162496745511</v>
+        <v>3747.081408254661</v>
       </c>
       <c r="M6" t="n">
-        <v>1482.348204437319</v>
+        <v>1478.616647725951</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -761,13 +761,13 @@
         <v>800</v>
       </c>
       <c r="B7" t="n">
-        <v>1.108814844013317</v>
+        <v>1.151402426919578</v>
       </c>
       <c r="C7" t="n">
-        <v>0.504104793960223</v>
+        <v>0.5136944600970971</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4937454950287892</v>
+        <v>0.5037685693587338</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -776,10 +776,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0893627025064106</v>
+        <v>0.0917610685447697</v>
       </c>
       <c r="H7" t="n">
-        <v>6.616615762249937</v>
+        <v>6.819795041725524</v>
       </c>
       <c r="I7" t="n">
         <v>480</v>
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>149.7722432865874</v>
+        <v>149.7917639966689</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -807,40 +807,40 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>788</v>
+        <v>777</v>
       </c>
       <c r="B8" t="n">
-        <v>35.60832764402537</v>
+        <v>35.11561962361235</v>
       </c>
       <c r="C8" t="n">
-        <v>2.878385679488622</v>
+        <v>2.878564492392675</v>
       </c>
       <c r="D8" t="n">
-        <v>2.878352272022043</v>
+        <v>2.878531130556662</v>
       </c>
       <c r="E8" t="n">
-        <v>22.63156511099816</v>
+        <v>22.63111160174193</v>
       </c>
       <c r="F8" t="n">
-        <v>22.5611222046088</v>
+        <v>22.56248150356302</v>
       </c>
       <c r="G8" t="n">
-        <v>2.837807283809311</v>
+        <v>2.798540895814356</v>
       </c>
       <c r="H8" t="n">
-        <v>106.7727279996163</v>
+        <v>105.2927433121898</v>
       </c>
       <c r="I8" t="n">
         <v>480</v>
       </c>
       <c r="J8" t="n">
-        <v>2.224431833325339</v>
+        <v>2.193598819003953</v>
       </c>
       <c r="K8" t="n">
         <v>5</v>
       </c>
       <c r="L8" t="n">
-        <v>515.27639072567</v>
+        <v>508.1504159660739</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -856,40 +856,40 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>780</v>
+        <v>763</v>
       </c>
       <c r="B9" t="n">
-        <v>83.75583623850962</v>
+        <v>82.11858239032379</v>
       </c>
       <c r="C9" t="n">
-        <v>4.437072689917541</v>
+        <v>4.442165738462506</v>
       </c>
       <c r="D9" t="n">
-        <v>4.436533133103275</v>
+        <v>4.441632988807243</v>
       </c>
       <c r="E9" t="n">
-        <v>36.01993997743721</v>
+        <v>36.02203883103742</v>
       </c>
       <c r="F9" t="n">
-        <v>35.95246892723667</v>
+        <v>35.95680124014695</v>
       </c>
       <c r="G9" t="n">
-        <v>4.684141845194391</v>
+        <v>4.588322905533941</v>
       </c>
       <c r="H9" t="n">
-        <v>211.6823046218628</v>
+        <v>207.4503275129931</v>
       </c>
       <c r="I9" t="n">
         <v>480</v>
       </c>
       <c r="J9" t="n">
-        <v>4.410048012955476</v>
+        <v>4.321881823187356</v>
       </c>
       <c r="K9" t="n">
         <v>10</v>
       </c>
       <c r="L9" t="n">
-        <v>1525.883831452433</v>
+        <v>1495.890735317712</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -905,43 +905,43 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>760</v>
+        <v>751</v>
       </c>
       <c r="B10" t="n">
-        <v>140.1946686297036</v>
+        <v>139.3622383003088</v>
       </c>
       <c r="C10" t="n">
-        <v>5.815609783013524</v>
+        <v>5.832958591087717</v>
       </c>
       <c r="D10" t="n">
-        <v>5.81226380655121</v>
+        <v>5.829649439338227</v>
       </c>
       <c r="E10" t="n">
-        <v>48.10490072181218</v>
+        <v>48.11454877754961</v>
       </c>
       <c r="F10" t="n">
-        <v>48.03521424812077</v>
+        <v>48.04658287481557</v>
       </c>
       <c r="G10" t="n">
-        <v>6.408250625216334</v>
+        <v>6.357301543717624</v>
       </c>
       <c r="H10" t="n">
-        <v>318.4116740688982</v>
+        <v>316.1488532056907</v>
       </c>
       <c r="I10" t="n">
         <v>480</v>
       </c>
       <c r="J10" t="n">
-        <v>6.633576543102045</v>
+        <v>6.586434441785224</v>
       </c>
       <c r="K10" t="n">
         <v>15</v>
       </c>
       <c r="L10" t="n">
-        <v>3228.943580924453</v>
+        <v>3209.655512182477</v>
       </c>
       <c r="M10" t="n">
-        <v>808.9975671116216</v>
+        <v>810.1570025813929</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -954,43 +954,43 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B11" t="n">
-        <v>190.2468369450918</v>
+        <v>190.303266909769</v>
       </c>
       <c r="C11" t="n">
-        <v>6.865610603790867</v>
+        <v>6.885262781597936</v>
       </c>
       <c r="D11" t="n">
-        <v>6.855817209189876</v>
+        <v>6.875513654645529</v>
       </c>
       <c r="E11" t="n">
-        <v>57.72035578985982</v>
+        <v>57.7301768256572</v>
       </c>
       <c r="F11" t="n">
-        <v>57.64696579013101</v>
+        <v>57.6570267755023</v>
       </c>
       <c r="G11" t="n">
-        <v>7.80948261759991</v>
+        <v>7.798246157536356</v>
       </c>
       <c r="H11" t="n">
-        <v>404.670722040429</v>
+        <v>404.3339878014114</v>
       </c>
       <c r="I11" t="n">
         <v>480</v>
       </c>
       <c r="J11" t="n">
-        <v>8.430640042508937</v>
+        <v>8.423624745862737</v>
       </c>
       <c r="K11" t="n">
         <v>20</v>
       </c>
       <c r="L11" t="n">
-        <v>5165.863206899546</v>
+        <v>5167.488790218209</v>
       </c>
       <c r="M11" t="n">
-        <v>1831.309494481392</v>
+        <v>1839.928815155501</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -1006,13 +1006,13 @@
         <v>500</v>
       </c>
       <c r="B12" t="n">
-        <v>0.7097087273788623</v>
+        <v>0.7137702800874285</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5101423472712506</v>
+        <v>0.5115999974410029</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5006763208460859</v>
+        <v>0.501725070229983</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -1021,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0.05656026916154987</v>
+        <v>0.05688395478855179</v>
       </c>
       <c r="H12" t="n">
-        <v>4.215165810632032</v>
+        <v>4.234513393189103</v>
       </c>
       <c r="I12" t="n">
         <v>480</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>93.61530651809927</v>
+        <v>93.61716819672704</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1052,28 +1052,28 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B13" t="n">
-        <v>13.66149265211713</v>
+        <v>13.76953395402863</v>
       </c>
       <c r="C13" t="n">
-        <v>2.265559491301191</v>
+        <v>2.265235580889897</v>
       </c>
       <c r="D13" t="n">
-        <v>2.265537789908774</v>
+        <v>2.265212596266086</v>
       </c>
       <c r="E13" t="n">
-        <v>17.95883087745015</v>
+        <v>17.95879625128244</v>
       </c>
       <c r="F13" t="n">
-        <v>17.90743091572676</v>
+        <v>17.90496140681934</v>
       </c>
       <c r="G13" t="n">
-        <v>1.088753275454349</v>
+        <v>1.097363631901914</v>
       </c>
       <c r="H13" t="n">
-        <v>45.02735668781079</v>
+        <v>45.38601674753248</v>
       </c>
       <c r="I13" t="n">
         <v>480</v>
@@ -1085,7 +1085,7 @@
         <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>203.1908928375152</v>
+        <v>204.8087256083742</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -1101,40 +1101,40 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B14" t="n">
-        <v>37.60861421634392</v>
+        <v>37.13373621317103</v>
       </c>
       <c r="C14" t="n">
-        <v>3.786233839707495</v>
+        <v>3.785940850933355</v>
       </c>
       <c r="D14" t="n">
-        <v>3.786163091925348</v>
+        <v>3.785866775246867</v>
       </c>
       <c r="E14" t="n">
-        <v>29.13355108743834</v>
+        <v>29.13301342225243</v>
       </c>
       <c r="F14" t="n">
-        <v>29.09072209493488</v>
+        <v>29.08828149323029</v>
       </c>
       <c r="G14" t="n">
-        <v>2.405982444478958</v>
+        <v>2.375764370630197</v>
       </c>
       <c r="H14" t="n">
-        <v>101.1970857237514</v>
+        <v>99.92234049449684</v>
       </c>
       <c r="I14" t="n">
         <v>480</v>
       </c>
       <c r="J14" t="n">
-        <v>2.108272619244821</v>
+        <v>2.081715426968684</v>
       </c>
       <c r="K14" t="n">
         <v>10</v>
       </c>
       <c r="L14" t="n">
-        <v>591.2383910659049</v>
+        <v>583.7458474443873</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1150,43 +1150,43 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="B15" t="n">
-        <v>73.34613919390094</v>
+        <v>71.89404937001953</v>
       </c>
       <c r="C15" t="n">
-        <v>5.343360564989762</v>
+        <v>5.347272486405408</v>
       </c>
       <c r="D15" t="n">
-        <v>5.34261332350262</v>
+        <v>5.346508437128667</v>
       </c>
       <c r="E15" t="n">
-        <v>38.74819224388952</v>
+        <v>38.7493746968496</v>
       </c>
       <c r="F15" t="n">
-        <v>38.70485285839883</v>
+        <v>38.70334980046432</v>
       </c>
       <c r="G15" t="n">
-        <v>3.558579304232819</v>
+        <v>3.486282886248371</v>
       </c>
       <c r="H15" t="n">
-        <v>172.2515541586773</v>
+        <v>168.7925567775223</v>
       </c>
       <c r="I15" t="n">
         <v>480</v>
       </c>
       <c r="J15" t="n">
-        <v>3.588574044972443</v>
+        <v>3.516511599531715</v>
       </c>
       <c r="K15" t="n">
         <v>15</v>
       </c>
       <c r="L15" t="n">
-        <v>1389.174233363995</v>
+        <v>1361.500772819123</v>
       </c>
       <c r="M15" t="n">
-        <v>260.1085609940858</v>
+        <v>255.5878685663937</v>
       </c>
       <c r="N15" t="n">
         <v>0</v>
@@ -1199,43 +1199,43 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="B16" t="n">
-        <v>114.0357859624557</v>
+        <v>111.012337533814</v>
       </c>
       <c r="C16" t="n">
-        <v>6.698289705021809</v>
+        <v>6.710466485806138</v>
       </c>
       <c r="D16" t="n">
-        <v>6.695183945154577</v>
+        <v>6.707368506691897</v>
       </c>
       <c r="E16" t="n">
-        <v>46.38782835256767</v>
+        <v>46.3931922815417</v>
       </c>
       <c r="F16" t="n">
-        <v>46.34310868893961</v>
+        <v>46.34522099789339</v>
       </c>
       <c r="G16" t="n">
-        <v>4.754599145553132</v>
+        <v>4.623335021611265</v>
       </c>
       <c r="H16" t="n">
-        <v>244.9390446995887</v>
+        <v>238.2739350045039</v>
       </c>
       <c r="I16" t="n">
         <v>480</v>
       </c>
       <c r="J16" t="n">
-        <v>5.102896764574765</v>
+        <v>4.964040312593832</v>
       </c>
       <c r="K16" t="n">
         <v>20</v>
       </c>
       <c r="L16" t="n">
-        <v>2509.481869528717</v>
+        <v>2442.758324069539</v>
       </c>
       <c r="M16" t="n">
-        <v>835.2558091584109</v>
+        <v>815.5289352177025</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -1251,13 +1251,13 @@
         <v>500</v>
       </c>
       <c r="B17" t="n">
-        <v>0.7139759457319661</v>
+        <v>0.687929221410262</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5116736982995517</v>
+        <v>0.5022537429819555</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5011958360357722</v>
+        <v>0.492733169036367</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -1266,10 +1266,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0.04555543824417715</v>
+        <v>0.04389351959216424</v>
       </c>
       <c r="H17" t="n">
-        <v>4.235492521224415</v>
+        <v>4.111040084573148</v>
       </c>
       <c r="I17" t="n">
         <v>490</v>
@@ -1281,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>93.61726246691443</v>
+        <v>93.60532352792423</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
@@ -1297,40 +1297,40 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B18" t="n">
-        <v>15.88487775465924</v>
+        <v>15.92202244767113</v>
       </c>
       <c r="C18" t="n">
-        <v>2.428089938803689</v>
+        <v>2.428470441920808</v>
       </c>
       <c r="D18" t="n">
-        <v>2.428065864610065</v>
+        <v>2.428446478652079</v>
       </c>
       <c r="E18" t="n">
-        <v>22.63597979397477</v>
+        <v>22.63625906182645</v>
       </c>
       <c r="F18" t="n">
-        <v>22.56474984441798</v>
+        <v>22.56831595571246</v>
       </c>
       <c r="G18" t="n">
-        <v>1.013539142172089</v>
+        <v>1.01590916987219</v>
       </c>
       <c r="H18" t="n">
-        <v>50.94210700952914</v>
+        <v>51.05806806878169</v>
       </c>
       <c r="I18" t="n">
         <v>490</v>
       </c>
       <c r="J18" t="n">
-        <v>1.039634836929166</v>
+        <v>1.04200138915881</v>
       </c>
       <c r="K18" t="n">
         <v>5</v>
       </c>
       <c r="L18" t="n">
-        <v>256.4730784900042</v>
+        <v>257.069849815854</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
@@ -1346,40 +1346,40 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B19" t="n">
-        <v>43.53876424850066</v>
+        <v>42.83804835625742</v>
       </c>
       <c r="C19" t="n">
-        <v>4.040358717115596</v>
+        <v>4.04090467497139</v>
       </c>
       <c r="D19" t="n">
-        <v>4.040292617158944</v>
+        <v>4.040836549491504</v>
       </c>
       <c r="E19" t="n">
-        <v>36.58705068699365</v>
+        <v>36.58707673776006</v>
       </c>
       <c r="F19" t="n">
-        <v>36.52717435545757</v>
+        <v>36.5294401713959</v>
       </c>
       <c r="G19" t="n">
-        <v>2.181206615019974</v>
+        <v>2.145886683648852</v>
       </c>
       <c r="H19" t="n">
-        <v>114.1859945062836</v>
+        <v>112.3422811871288</v>
       </c>
       <c r="I19" t="n">
         <v>490</v>
       </c>
       <c r="J19" t="n">
-        <v>2.330326418495584</v>
+        <v>2.292699616063854</v>
       </c>
       <c r="K19" t="n">
         <v>10</v>
       </c>
       <c r="L19" t="n">
-        <v>820.2176909545979</v>
+        <v>807.0372324284087</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
@@ -1395,43 +1395,43 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="B20" t="n">
-        <v>80.53360913027667</v>
+        <v>79.25932786285384</v>
       </c>
       <c r="C20" t="n">
-        <v>5.529060234636172</v>
+        <v>5.536971996804944</v>
       </c>
       <c r="D20" t="n">
-        <v>5.528483722153019</v>
+        <v>5.536372678018728</v>
       </c>
       <c r="E20" t="n">
-        <v>50.11204232546336</v>
+        <v>50.11560307827571</v>
       </c>
       <c r="F20" t="n">
-        <v>50.05203522753623</v>
+        <v>50.0578465482267</v>
       </c>
       <c r="G20" t="n">
-        <v>3.269346220664115</v>
+        <v>3.214844027538497</v>
       </c>
       <c r="H20" t="n">
-        <v>186.5960737647942</v>
+        <v>183.5398729037619</v>
       </c>
       <c r="I20" t="n">
         <v>490</v>
       </c>
       <c r="J20" t="n">
-        <v>3.808083138057024</v>
+        <v>3.745711691913507</v>
       </c>
       <c r="K20" t="n">
         <v>15</v>
       </c>
       <c r="L20" t="n">
-        <v>1937.812717192857</v>
+        <v>1907.107672888115</v>
       </c>
       <c r="M20" t="n">
-        <v>425.0448510757132</v>
+        <v>420.0997541497803</v>
       </c>
       <c r="N20" t="n">
         <v>0</v>
@@ -1444,43 +1444,43 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B21" t="n">
-        <v>117.0406322993006</v>
+        <v>118.2477830309855</v>
       </c>
       <c r="C21" t="n">
-        <v>6.77869657670941</v>
+        <v>6.799021078141265</v>
       </c>
       <c r="D21" t="n">
-        <v>6.776519740489332</v>
+        <v>6.796704856080432</v>
       </c>
       <c r="E21" t="n">
-        <v>63.46518167680613</v>
+        <v>63.47513064507812</v>
       </c>
       <c r="F21" t="n">
-        <v>63.40262987951647</v>
+        <v>63.41420701930006</v>
       </c>
       <c r="G21" t="n">
-        <v>4.238573924850392</v>
+        <v>4.275609357765627</v>
       </c>
       <c r="H21" t="n">
-        <v>250.2110717470139</v>
+        <v>252.4929722765037</v>
       </c>
       <c r="I21" t="n">
         <v>490</v>
       </c>
       <c r="J21" t="n">
-        <v>5.106348403000284</v>
+        <v>5.1529178015613</v>
       </c>
       <c r="K21" t="n">
         <v>20</v>
       </c>
       <c r="L21" t="n">
-        <v>3488.727379834837</v>
+        <v>3524.813103493363</v>
       </c>
       <c r="M21" t="n">
-        <v>1219.960272798553</v>
+        <v>1238.449764534581</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
@@ -1552,16 +1552,16 @@
         <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D2" t="n">
-        <v>3759.162496745511</v>
+        <v>3747.081408254661</v>
       </c>
       <c r="E2" t="n">
-        <v>7.401643667966121</v>
+        <v>7.405522824688475</v>
       </c>
       <c r="F2" t="n">
-        <v>57.95362926591102</v>
+        <v>57.95892898370582</v>
       </c>
     </row>
     <row r="3">
@@ -1574,16 +1574,16 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="D3" t="n">
-        <v>5165.863206899546</v>
+        <v>5167.488790218209</v>
       </c>
       <c r="E3" t="n">
-        <v>6.855817209189876</v>
+        <v>6.875513654645529</v>
       </c>
       <c r="F3" t="n">
-        <v>57.64696579013101</v>
+        <v>57.6570267755023</v>
       </c>
     </row>
     <row r="4">
@@ -1596,16 +1596,16 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="D4" t="n">
-        <v>2509.481869528717</v>
+        <v>2442.758324069539</v>
       </c>
       <c r="E4" t="n">
-        <v>6.695183945154577</v>
+        <v>6.707368506691897</v>
       </c>
       <c r="F4" t="n">
-        <v>46.34310868893961</v>
+        <v>46.34522099789339</v>
       </c>
     </row>
     <row r="5">
@@ -1618,16 +1618,16 @@
         <v>20</v>
       </c>
       <c r="C5" t="n">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D5" t="n">
-        <v>3488.727379834837</v>
+        <v>3524.813103493363</v>
       </c>
       <c r="E5" t="n">
-        <v>6.776519740489332</v>
+        <v>6.796704856080432</v>
       </c>
       <c r="F5" t="n">
-        <v>63.40262987951647</v>
+        <v>63.41420701930006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>